<commit_message>
Internship task list with progress
</commit_message>
<xml_diff>
--- a/AnkitaTapaseQATesting internship.xlsx
+++ b/AnkitaTapaseQATesting internship.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software-Testing-Course\Internship-Assignment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D893D38-659A-4435-8915-254C1F5E25A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Task" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -973,54 +982,56 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15.0"/>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="15.0"/>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -1031,62 +1042,59 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1276,31 +1284,61 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z336"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="C224" sqref="C224"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.75"/>
-    <col customWidth="1" min="2" max="2" width="51.5"/>
-    <col customWidth="1" min="3" max="3" width="50.38"/>
-    <col customWidth="1" min="4" max="4" width="57.5"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1330,7 +1368,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1366,7 +1404,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1380,7 +1418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1408,7 +1446,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1422,7 +1460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -1436,7 +1474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1450,7 +1488,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1464,7 +1502,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1478,7 +1516,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
@@ -1492,7 +1530,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>42</v>
       </c>
@@ -1506,7 +1544,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1536,7 +1574,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -1549,9 +1587,9 @@
       <c r="D16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -1564,9 +1602,9 @@
       <c r="D17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>51</v>
       </c>
@@ -1579,9 +1617,9 @@
       <c r="D18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>55</v>
       </c>
@@ -1594,9 +1632,9 @@
       <c r="D19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>59</v>
       </c>
@@ -1609,9 +1647,9 @@
       <c r="D20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>63</v>
       </c>
@@ -1624,9 +1662,9 @@
       <c r="D21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="23">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="23" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
@@ -1656,7 +1694,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>2</v>
       </c>
@@ -1670,7 +1708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>68</v>
       </c>
@@ -1684,7 +1722,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>72</v>
       </c>
@@ -1698,7 +1736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>76</v>
       </c>
@@ -1712,7 +1750,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>80</v>
       </c>
@@ -1726,7 +1764,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>84</v>
       </c>
@@ -1756,7 +1794,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>2</v>
       </c>
@@ -1770,7 +1808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>85</v>
       </c>
@@ -1784,7 +1822,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>89</v>
       </c>
@@ -1798,7 +1836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>93</v>
       </c>
@@ -1812,7 +1850,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>97</v>
       </c>
@@ -1826,7 +1864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>101</v>
       </c>
@@ -1856,348 +1894,348 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-    </row>
-    <row r="40">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-    </row>
-    <row r="43">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="8" t="s">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
-      <c r="N53" s="9"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
-      <c r="Q53" s="9"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="9"/>
-      <c r="T53" s="9"/>
-      <c r="U53" s="9"/>
-      <c r="V53" s="9"/>
-      <c r="W53" s="9"/>
-      <c r="X53" s="9"/>
-      <c r="Y53" s="9"/>
-      <c r="Z53" s="9"/>
-    </row>
-    <row r="54">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+    </row>
+    <row r="54" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
-      <c r="L54" s="10"/>
-      <c r="M54" s="10"/>
-      <c r="N54" s="10"/>
-      <c r="O54" s="10"/>
-      <c r="P54" s="10"/>
-      <c r="Q54" s="10"/>
-      <c r="R54" s="10"/>
-      <c r="S54" s="10"/>
-      <c r="T54" s="10"/>
-      <c r="U54" s="10"/>
-      <c r="V54" s="10"/>
-      <c r="W54" s="10"/>
-      <c r="X54" s="10"/>
-      <c r="Y54" s="10"/>
-      <c r="Z54" s="10"/>
-    </row>
-    <row r="55">
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="11" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+    </row>
+    <row r="55" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57">
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="11" t="s">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="11" t="s">
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="11" t="s">
+    <row r="60" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="11" t="s">
+    <row r="61" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="11" t="s">
+    <row r="62" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="11" t="s">
+    <row r="63" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="11" t="s">
+    <row r="65" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="11" t="s">
+    <row r="67" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="11" t="s">
+    <row r="68" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="11" t="s">
+    <row r="69" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="11" t="s">
+    <row r="70" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="11" t="s">
+    <row r="72" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="11" t="s">
+    <row r="74" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="11" t="s">
+    <row r="75" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="11" t="s">
+    <row r="76" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="11" t="s">
+    <row r="77" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="11" t="s">
+    <row r="78" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="11" t="s">
+    <row r="79" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="11" t="s">
+    <row r="81" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="11" t="s">
+    <row r="83" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="11" t="s">
+    <row r="84" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="11" t="s">
+    <row r="85" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="11" t="s">
+    <row r="86" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="11" t="s">
+    <row r="87" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-      <c r="I89" s="10"/>
-      <c r="J89" s="10"/>
-      <c r="K89" s="10"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="10"/>
-      <c r="Q89" s="10"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="10"/>
-      <c r="T89" s="10"/>
-      <c r="U89" s="10"/>
-      <c r="V89" s="10"/>
-      <c r="W89" s="10"/>
-      <c r="X89" s="10"/>
-      <c r="Y89" s="10"/>
-      <c r="Z89" s="10"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="11" t="s">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+      <c r="P89" s="2"/>
+      <c r="Q89" s="2"/>
+      <c r="R89" s="2"/>
+      <c r="S89" s="2"/>
+      <c r="T89" s="2"/>
+      <c r="U89" s="2"/>
+      <c r="V89" s="2"/>
+      <c r="W89" s="2"/>
+      <c r="X89" s="2"/>
+      <c r="Y89" s="2"/>
+      <c r="Z89" s="2"/>
+    </row>
+    <row r="91" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="12" t="s">
+    <row r="93" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C93" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E93" s="5"/>
@@ -2223,64 +2261,64 @@
       <c r="Y93" s="5"/>
       <c r="Z93" s="5"/>
     </row>
-    <row r="94">
-      <c r="A94" s="11" t="s">
+    <row r="94" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D94" s="11" t="s">
+      <c r="D94" s="7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="11" t="s">
+    <row r="95" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D95" s="11" t="s">
+      <c r="D95" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="11" t="s">
+    <row r="96" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="B96" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D96" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="11" t="s">
+    <row r="98" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A98" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="12" t="s">
+    <row r="100" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B100" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C100" s="12" t="s">
+      <c r="C100" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E100" s="5"/>
@@ -2306,64 +2344,64 @@
       <c r="Y100" s="5"/>
       <c r="Z100" s="5"/>
     </row>
-    <row r="101">
-      <c r="A101" s="11" t="s">
+    <row r="101" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A101" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D101" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="11" t="s">
+    <row r="102" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A102" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D102" s="11" t="s">
+      <c r="D102" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="11" t="s">
+    <row r="103" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A103" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D103" s="11" t="s">
+      <c r="D103" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="11" t="s">
+    <row r="105" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A105" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="12" t="s">
+    <row r="107" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C107" s="12" t="s">
+      <c r="C107" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E107" s="5"/>
@@ -2389,64 +2427,64 @@
       <c r="Y107" s="5"/>
       <c r="Z107" s="5"/>
     </row>
-    <row r="108">
-      <c r="A108" s="11" t="s">
+    <row r="108" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A108" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D108" s="11" t="s">
+      <c r="D108" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="11" t="s">
+    <row r="109" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B109" s="11" t="s">
+      <c r="B109" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D109" s="11" t="s">
+      <c r="D109" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="11" t="s">
+    <row r="110" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D110" s="11" t="s">
+      <c r="D110" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="11" t="s">
+    <row r="112" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A112" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="12" t="s">
+    <row r="114" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B114" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="12" t="s">
+      <c r="C114" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E114" s="5"/>
@@ -2472,164 +2510,164 @@
       <c r="Y114" s="5"/>
       <c r="Z114" s="5"/>
     </row>
-    <row r="115">
-      <c r="A115" s="11" t="s">
+    <row r="115" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B115" s="11" t="s">
+      <c r="B115" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D115" s="11" t="s">
+      <c r="D115" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="11" t="s">
+    <row r="116" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A116" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D116" s="11" t="s">
+      <c r="D116" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="11" t="s">
+    <row r="117" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A117" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="B117" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C117" s="11" t="s">
+      <c r="C117" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D117" s="11" t="s">
+      <c r="D117" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B119" s="10"/>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="10"/>
-      <c r="F119" s="10"/>
-      <c r="G119" s="10"/>
-      <c r="H119" s="10"/>
-      <c r="I119" s="10"/>
-      <c r="J119" s="10"/>
-      <c r="K119" s="10"/>
-      <c r="L119" s="10"/>
-      <c r="M119" s="10"/>
-      <c r="N119" s="10"/>
-      <c r="O119" s="10"/>
-      <c r="P119" s="10"/>
-      <c r="Q119" s="10"/>
-      <c r="R119" s="10"/>
-      <c r="S119" s="10"/>
-      <c r="T119" s="10"/>
-      <c r="U119" s="10"/>
-      <c r="V119" s="10"/>
-      <c r="W119" s="10"/>
-      <c r="X119" s="10"/>
-      <c r="Y119" s="10"/>
-      <c r="Z119" s="10"/>
-    </row>
-    <row r="121">
-      <c r="A121" s="11" t="s">
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+      <c r="L119" s="2"/>
+      <c r="M119" s="2"/>
+      <c r="N119" s="2"/>
+      <c r="O119" s="2"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="2"/>
+      <c r="R119" s="2"/>
+      <c r="S119" s="2"/>
+      <c r="T119" s="2"/>
+      <c r="U119" s="2"/>
+      <c r="V119" s="2"/>
+      <c r="W119" s="2"/>
+      <c r="X119" s="2"/>
+      <c r="Y119" s="2"/>
+      <c r="Z119" s="2"/>
+    </row>
+    <row r="121" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A121" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B123" s="10"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="10"/>
-      <c r="G123" s="10"/>
-      <c r="H123" s="10"/>
-      <c r="I123" s="10"/>
-      <c r="J123" s="10"/>
-      <c r="K123" s="10"/>
-      <c r="L123" s="10"/>
-      <c r="M123" s="10"/>
-      <c r="N123" s="10"/>
-      <c r="O123" s="10"/>
-      <c r="P123" s="10"/>
-      <c r="Q123" s="10"/>
-      <c r="R123" s="10"/>
-      <c r="S123" s="10"/>
-      <c r="T123" s="10"/>
-      <c r="U123" s="10"/>
-      <c r="V123" s="10"/>
-      <c r="W123" s="10"/>
-      <c r="X123" s="10"/>
-      <c r="Y123" s="10"/>
-      <c r="Z123" s="10"/>
-    </row>
-    <row r="125">
-      <c r="A125" s="11" t="s">
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+      <c r="N123" s="2"/>
+      <c r="O123" s="2"/>
+      <c r="P123" s="2"/>
+      <c r="Q123" s="2"/>
+      <c r="R123" s="2"/>
+      <c r="S123" s="2"/>
+      <c r="T123" s="2"/>
+      <c r="U123" s="2"/>
+      <c r="V123" s="2"/>
+      <c r="W123" s="2"/>
+      <c r="X123" s="2"/>
+      <c r="Y123" s="2"/>
+      <c r="Z123" s="2"/>
+    </row>
+    <row r="125" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A125" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="11" t="s">
+    <row r="127" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A127" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" s="11" t="s">
+    <row r="129" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A129" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" s="11" t="s">
+    <row r="130" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A130" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" s="8" t="s">
+    <row r="132" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B132" s="9"/>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9"/>
-      <c r="E132" s="9"/>
-      <c r="F132" s="9"/>
-      <c r="G132" s="9"/>
-      <c r="H132" s="9"/>
-      <c r="I132" s="9"/>
-      <c r="J132" s="9"/>
-      <c r="K132" s="9"/>
-      <c r="L132" s="9"/>
-      <c r="M132" s="9"/>
-      <c r="N132" s="9"/>
-      <c r="O132" s="9"/>
-      <c r="P132" s="9"/>
-      <c r="Q132" s="9"/>
-      <c r="R132" s="9"/>
-      <c r="S132" s="9"/>
-      <c r="T132" s="9"/>
-      <c r="U132" s="9"/>
-      <c r="V132" s="9"/>
-      <c r="W132" s="9"/>
-      <c r="X132" s="9"/>
-      <c r="Y132" s="9"/>
-      <c r="Z132" s="9"/>
-    </row>
-    <row r="134">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+      <c r="Q132" s="1"/>
+      <c r="R132" s="1"/>
+      <c r="S132" s="1"/>
+      <c r="T132" s="1"/>
+      <c r="U132" s="1"/>
+      <c r="V132" s="1"/>
+      <c r="W132" s="1"/>
+      <c r="X132" s="1"/>
+      <c r="Y132" s="1"/>
+      <c r="Z132" s="1"/>
+    </row>
+    <row r="134" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>199</v>
       </c>
@@ -2659,1491 +2697,1491 @@
       <c r="Y134" s="3"/>
       <c r="Z134" s="3"/>
     </row>
-    <row r="135">
-      <c r="A135" s="13"/>
-    </row>
-    <row r="136">
+    <row r="135" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="A135" s="9"/>
+    </row>
+    <row r="136" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B136" s="7"/>
-      <c r="C136" s="7"/>
-    </row>
-    <row r="137">
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B137" s="7"/>
-      <c r="C137" s="7"/>
-    </row>
-    <row r="138">
-      <c r="A138" s="7"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
-    </row>
-    <row r="139">
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+    </row>
+    <row r="138" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A138" s="6"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+    </row>
+    <row r="139" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-    </row>
-    <row r="140">
-      <c r="A140" s="7"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
-    </row>
-    <row r="141">
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+    </row>
+    <row r="140" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+    </row>
+    <row r="141" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
-    </row>
-    <row r="142">
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+    </row>
+    <row r="142" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
-    </row>
-    <row r="143">
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+    </row>
+    <row r="143" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
-    </row>
-    <row r="144">
-      <c r="A144" s="7"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
-    </row>
-    <row r="145">
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A144" s="6"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+    </row>
+    <row r="145" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B145" s="10"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="10"/>
-      <c r="E145" s="10"/>
-      <c r="F145" s="10"/>
-      <c r="G145" s="10"/>
-      <c r="H145" s="10"/>
-      <c r="I145" s="10"/>
-      <c r="J145" s="10"/>
-      <c r="K145" s="10"/>
-      <c r="L145" s="10"/>
-      <c r="M145" s="10"/>
-      <c r="N145" s="10"/>
-      <c r="O145" s="10"/>
-      <c r="P145" s="10"/>
-      <c r="Q145" s="10"/>
-      <c r="R145" s="10"/>
-      <c r="S145" s="10"/>
-      <c r="T145" s="10"/>
-      <c r="U145" s="10"/>
-      <c r="V145" s="10"/>
-      <c r="W145" s="10"/>
-      <c r="X145" s="10"/>
-      <c r="Y145" s="10"/>
-      <c r="Z145" s="10"/>
-    </row>
-    <row r="146">
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+      <c r="L145" s="2"/>
+      <c r="M145" s="2"/>
+      <c r="N145" s="2"/>
+      <c r="O145" s="2"/>
+      <c r="P145" s="2"/>
+      <c r="Q145" s="2"/>
+      <c r="R145" s="2"/>
+      <c r="S145" s="2"/>
+      <c r="T145" s="2"/>
+      <c r="U145" s="2"/>
+      <c r="V145" s="2"/>
+      <c r="W145" s="2"/>
+      <c r="X145" s="2"/>
+      <c r="Y145" s="2"/>
+      <c r="Z145" s="2"/>
+    </row>
+    <row r="146" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-    </row>
-    <row r="147">
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B147" s="7"/>
-      <c r="C147" s="7"/>
-    </row>
-    <row r="148">
-      <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
-      <c r="C148" s="7"/>
-    </row>
-    <row r="149">
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B149" s="7"/>
-      <c r="C149" s="7"/>
-    </row>
-    <row r="150">
-      <c r="A150" s="7"/>
-      <c r="B150" s="7"/>
-      <c r="C150" s="7"/>
-    </row>
-    <row r="151">
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+    </row>
+    <row r="151" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
-    </row>
-    <row r="152">
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A152" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B152" s="7"/>
-      <c r="C152" s="7"/>
-    </row>
-    <row r="153">
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+    </row>
+    <row r="153" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A153" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
-    </row>
-    <row r="154">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-    </row>
-    <row r="155">
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+    </row>
+    <row r="154" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+    </row>
+    <row r="155" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B155" s="10"/>
-      <c r="C155" s="10"/>
-      <c r="D155" s="10"/>
-      <c r="E155" s="10"/>
-      <c r="F155" s="10"/>
-      <c r="G155" s="10"/>
-      <c r="H155" s="10"/>
-      <c r="I155" s="10"/>
-      <c r="J155" s="10"/>
-      <c r="K155" s="10"/>
-      <c r="L155" s="10"/>
-      <c r="M155" s="10"/>
-      <c r="N155" s="10"/>
-      <c r="O155" s="10"/>
-      <c r="P155" s="10"/>
-      <c r="Q155" s="10"/>
-      <c r="R155" s="10"/>
-      <c r="S155" s="10"/>
-      <c r="T155" s="10"/>
-      <c r="U155" s="10"/>
-      <c r="V155" s="10"/>
-      <c r="W155" s="10"/>
-      <c r="X155" s="10"/>
-      <c r="Y155" s="10"/>
-      <c r="Z155" s="10"/>
-    </row>
-    <row r="156">
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+      <c r="L155" s="2"/>
+      <c r="M155" s="2"/>
+      <c r="N155" s="2"/>
+      <c r="O155" s="2"/>
+      <c r="P155" s="2"/>
+      <c r="Q155" s="2"/>
+      <c r="R155" s="2"/>
+      <c r="S155" s="2"/>
+      <c r="T155" s="2"/>
+      <c r="U155" s="2"/>
+      <c r="V155" s="2"/>
+      <c r="W155" s="2"/>
+      <c r="X155" s="2"/>
+      <c r="Y155" s="2"/>
+      <c r="Z155" s="2"/>
+    </row>
+    <row r="156" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A156" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B156" s="7"/>
-      <c r="C156" s="7"/>
-    </row>
-    <row r="157">
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+    </row>
+    <row r="157" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A157" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-    </row>
-    <row r="158">
-      <c r="A158" s="7"/>
-      <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
-    </row>
-    <row r="159">
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+    </row>
+    <row r="158" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+    </row>
+    <row r="159" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-    </row>
-    <row r="160">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-    </row>
-    <row r="161">
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+    </row>
+    <row r="160" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+    </row>
+    <row r="161" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A161" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B161" s="7"/>
-      <c r="C161" s="7"/>
-    </row>
-    <row r="162">
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+    </row>
+    <row r="162" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A162" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B162" s="7"/>
-      <c r="C162" s="7"/>
-    </row>
-    <row r="163">
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+    </row>
+    <row r="163" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A163" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B163" s="7"/>
-      <c r="C163" s="7"/>
-    </row>
-    <row r="164">
-      <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="7"/>
-    </row>
-    <row r="165">
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+    </row>
+    <row r="164" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+    </row>
+    <row r="165" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B165" s="10"/>
-      <c r="C165" s="10"/>
-      <c r="D165" s="10"/>
-      <c r="E165" s="10"/>
-      <c r="F165" s="10"/>
-      <c r="G165" s="10"/>
-      <c r="H165" s="10"/>
-      <c r="I165" s="10"/>
-      <c r="J165" s="10"/>
-      <c r="K165" s="10"/>
-      <c r="L165" s="10"/>
-      <c r="M165" s="10"/>
-      <c r="N165" s="10"/>
-      <c r="O165" s="10"/>
-      <c r="P165" s="10"/>
-      <c r="Q165" s="10"/>
-      <c r="R165" s="10"/>
-      <c r="S165" s="10"/>
-      <c r="T165" s="10"/>
-      <c r="U165" s="10"/>
-      <c r="V165" s="10"/>
-      <c r="W165" s="10"/>
-      <c r="X165" s="10"/>
-      <c r="Y165" s="10"/>
-      <c r="Z165" s="10"/>
-    </row>
-    <row r="166">
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+      <c r="J165" s="2"/>
+      <c r="K165" s="2"/>
+      <c r="L165" s="2"/>
+      <c r="M165" s="2"/>
+      <c r="N165" s="2"/>
+      <c r="O165" s="2"/>
+      <c r="P165" s="2"/>
+      <c r="Q165" s="2"/>
+      <c r="R165" s="2"/>
+      <c r="S165" s="2"/>
+      <c r="T165" s="2"/>
+      <c r="U165" s="2"/>
+      <c r="V165" s="2"/>
+      <c r="W165" s="2"/>
+      <c r="X165" s="2"/>
+      <c r="Y165" s="2"/>
+      <c r="Z165" s="2"/>
+    </row>
+    <row r="166" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B166" s="7"/>
-      <c r="C166" s="7"/>
-    </row>
-    <row r="167">
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+    </row>
+    <row r="167" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B167" s="7"/>
-      <c r="C167" s="7"/>
-    </row>
-    <row r="168">
-      <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
-      <c r="C168" s="7"/>
-    </row>
-    <row r="169">
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+    </row>
+    <row r="168" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+    </row>
+    <row r="169" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B169" s="7"/>
-      <c r="C169" s="7"/>
-    </row>
-    <row r="170">
-      <c r="A170" s="7"/>
-      <c r="B170" s="7"/>
-      <c r="C170" s="7"/>
-    </row>
-    <row r="171">
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+    </row>
+    <row r="170" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+    </row>
+    <row r="171" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B171" s="7"/>
-      <c r="C171" s="7"/>
-    </row>
-    <row r="172">
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+    </row>
+    <row r="172" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B172" s="7"/>
-      <c r="C172" s="7"/>
-    </row>
-    <row r="173">
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+    </row>
+    <row r="173" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B173" s="7"/>
-      <c r="C173" s="7"/>
-    </row>
-    <row r="174">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="7"/>
-    </row>
-    <row r="175">
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+    </row>
+    <row r="174" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+    </row>
+    <row r="175" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B175" s="10"/>
-      <c r="C175" s="10"/>
-      <c r="D175" s="10"/>
-      <c r="E175" s="10"/>
-      <c r="F175" s="10"/>
-      <c r="G175" s="10"/>
-      <c r="H175" s="10"/>
-      <c r="I175" s="10"/>
-      <c r="J175" s="10"/>
-      <c r="K175" s="10"/>
-      <c r="L175" s="10"/>
-      <c r="M175" s="10"/>
-      <c r="N175" s="10"/>
-      <c r="O175" s="10"/>
-      <c r="P175" s="10"/>
-      <c r="Q175" s="10"/>
-      <c r="R175" s="10"/>
-      <c r="S175" s="10"/>
-      <c r="T175" s="10"/>
-      <c r="U175" s="10"/>
-      <c r="V175" s="10"/>
-      <c r="W175" s="10"/>
-      <c r="X175" s="10"/>
-      <c r="Y175" s="10"/>
-      <c r="Z175" s="10"/>
-    </row>
-    <row r="176">
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="2"/>
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+      <c r="J175" s="2"/>
+      <c r="K175" s="2"/>
+      <c r="L175" s="2"/>
+      <c r="M175" s="2"/>
+      <c r="N175" s="2"/>
+      <c r="O175" s="2"/>
+      <c r="P175" s="2"/>
+      <c r="Q175" s="2"/>
+      <c r="R175" s="2"/>
+      <c r="S175" s="2"/>
+      <c r="T175" s="2"/>
+      <c r="U175" s="2"/>
+      <c r="V175" s="2"/>
+      <c r="W175" s="2"/>
+      <c r="X175" s="2"/>
+      <c r="Y175" s="2"/>
+      <c r="Z175" s="2"/>
+    </row>
+    <row r="176" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A176" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B176" s="7"/>
-      <c r="C176" s="7"/>
-    </row>
-    <row r="177">
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+    </row>
+    <row r="177" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A177" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B177" s="7"/>
-      <c r="C177" s="7"/>
-    </row>
-    <row r="178">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
-      <c r="C178" s="7"/>
-    </row>
-    <row r="179">
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+    </row>
+    <row r="178" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+    </row>
+    <row r="179" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A179" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B179" s="7"/>
-      <c r="C179" s="7"/>
-    </row>
-    <row r="180">
-      <c r="A180" s="7"/>
-      <c r="B180" s="7"/>
-      <c r="C180" s="7"/>
-    </row>
-    <row r="181">
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+    </row>
+    <row r="180" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+    </row>
+    <row r="181" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A181" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
-    </row>
-    <row r="182">
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+    </row>
+    <row r="182" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A182" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B182" s="7"/>
-      <c r="C182" s="7"/>
-    </row>
-    <row r="183">
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+    </row>
+    <row r="183" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A183" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B183" s="7"/>
-      <c r="C183" s="7"/>
-    </row>
-    <row r="184">
-      <c r="A184" s="7"/>
-      <c r="B184" s="7"/>
-      <c r="C184" s="7"/>
-    </row>
-    <row r="185">
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+    </row>
+    <row r="184" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A184" s="6"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+    </row>
+    <row r="185" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B185" s="10"/>
-      <c r="C185" s="10"/>
-      <c r="D185" s="10"/>
-      <c r="E185" s="10"/>
-      <c r="F185" s="10"/>
-      <c r="G185" s="10"/>
-      <c r="H185" s="10"/>
-      <c r="I185" s="10"/>
-      <c r="J185" s="10"/>
-      <c r="K185" s="10"/>
-      <c r="L185" s="10"/>
-      <c r="M185" s="10"/>
-      <c r="N185" s="10"/>
-      <c r="O185" s="10"/>
-      <c r="P185" s="10"/>
-      <c r="Q185" s="10"/>
-      <c r="R185" s="10"/>
-      <c r="S185" s="10"/>
-      <c r="T185" s="10"/>
-      <c r="U185" s="10"/>
-      <c r="V185" s="10"/>
-      <c r="W185" s="10"/>
-      <c r="X185" s="10"/>
-      <c r="Y185" s="10"/>
-      <c r="Z185" s="10"/>
-    </row>
-    <row r="186">
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="2"/>
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+      <c r="J185" s="2"/>
+      <c r="K185" s="2"/>
+      <c r="L185" s="2"/>
+      <c r="M185" s="2"/>
+      <c r="N185" s="2"/>
+      <c r="O185" s="2"/>
+      <c r="P185" s="2"/>
+      <c r="Q185" s="2"/>
+      <c r="R185" s="2"/>
+      <c r="S185" s="2"/>
+      <c r="T185" s="2"/>
+      <c r="U185" s="2"/>
+      <c r="V185" s="2"/>
+      <c r="W185" s="2"/>
+      <c r="X185" s="2"/>
+      <c r="Y185" s="2"/>
+      <c r="Z185" s="2"/>
+    </row>
+    <row r="186" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A186" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B186" s="7"/>
-      <c r="C186" s="7"/>
-    </row>
-    <row r="187">
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+    </row>
+    <row r="187" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="B187" s="7"/>
-      <c r="C187" s="7"/>
-    </row>
-    <row r="188">
-      <c r="A188" s="7"/>
-      <c r="B188" s="7"/>
-      <c r="C188" s="7"/>
-    </row>
-    <row r="189">
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
+    </row>
+    <row r="188" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A188" s="6"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
+    </row>
+    <row r="189" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A189" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B189" s="7"/>
-      <c r="C189" s="7"/>
-    </row>
-    <row r="190">
-      <c r="A190" s="7"/>
-      <c r="B190" s="7"/>
-      <c r="C190" s="7"/>
-    </row>
-    <row r="191">
+      <c r="B189" s="6"/>
+      <c r="C189" s="6"/>
+    </row>
+    <row r="190" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A191" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B191" s="7"/>
-      <c r="C191" s="7"/>
-    </row>
-    <row r="192">
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+    </row>
+    <row r="192" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A192" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B192" s="7"/>
-      <c r="C192" s="7"/>
-    </row>
-    <row r="193">
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
+    </row>
+    <row r="193" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A193" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="B193" s="7"/>
-      <c r="C193" s="7"/>
-    </row>
-    <row r="194">
-      <c r="A194" s="7"/>
-      <c r="B194" s="7"/>
-      <c r="C194" s="7"/>
-    </row>
-    <row r="195">
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+    </row>
+    <row r="194" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+    </row>
+    <row r="195" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B195" s="10"/>
-      <c r="C195" s="10"/>
-      <c r="D195" s="10"/>
-      <c r="E195" s="10"/>
-      <c r="F195" s="10"/>
-      <c r="G195" s="10"/>
-      <c r="H195" s="10"/>
-      <c r="I195" s="10"/>
-      <c r="J195" s="10"/>
-      <c r="K195" s="10"/>
-      <c r="L195" s="10"/>
-      <c r="M195" s="10"/>
-      <c r="N195" s="10"/>
-      <c r="O195" s="10"/>
-      <c r="P195" s="10"/>
-      <c r="Q195" s="10"/>
-      <c r="R195" s="10"/>
-      <c r="S195" s="10"/>
-      <c r="T195" s="10"/>
-      <c r="U195" s="10"/>
-      <c r="V195" s="10"/>
-      <c r="W195" s="10"/>
-      <c r="X195" s="10"/>
-      <c r="Y195" s="10"/>
-      <c r="Z195" s="10"/>
-    </row>
-    <row r="196">
+      <c r="B195" s="2"/>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
+      <c r="E195" s="2"/>
+      <c r="F195" s="2"/>
+      <c r="G195" s="2"/>
+      <c r="H195" s="2"/>
+      <c r="I195" s="2"/>
+      <c r="J195" s="2"/>
+      <c r="K195" s="2"/>
+      <c r="L195" s="2"/>
+      <c r="M195" s="2"/>
+      <c r="N195" s="2"/>
+      <c r="O195" s="2"/>
+      <c r="P195" s="2"/>
+      <c r="Q195" s="2"/>
+      <c r="R195" s="2"/>
+      <c r="S195" s="2"/>
+      <c r="T195" s="2"/>
+      <c r="U195" s="2"/>
+      <c r="V195" s="2"/>
+      <c r="W195" s="2"/>
+      <c r="X195" s="2"/>
+      <c r="Y195" s="2"/>
+      <c r="Z195" s="2"/>
+    </row>
+    <row r="196" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B196" s="7"/>
-      <c r="C196" s="7"/>
-    </row>
-    <row r="197">
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+    </row>
+    <row r="197" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B197" s="7"/>
-      <c r="C197" s="7"/>
-    </row>
-    <row r="198">
-      <c r="A198" s="7"/>
-      <c r="B198" s="7"/>
-      <c r="C198" s="7"/>
-    </row>
-    <row r="199">
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+    </row>
+    <row r="198" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+    </row>
+    <row r="199" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B199" s="7"/>
-      <c r="C199" s="7"/>
-    </row>
-    <row r="200">
-      <c r="A200" s="7"/>
-      <c r="B200" s="7"/>
-      <c r="C200" s="7"/>
-    </row>
-    <row r="201">
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
+    </row>
+    <row r="200" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
+    </row>
+    <row r="201" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B201" s="7"/>
-      <c r="C201" s="7"/>
-    </row>
-    <row r="202">
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+    </row>
+    <row r="202" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A202" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B202" s="7"/>
-      <c r="C202" s="7"/>
-    </row>
-    <row r="203">
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
+    </row>
+    <row r="203" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="B203" s="7"/>
-      <c r="C203" s="7"/>
-    </row>
-    <row r="204">
-      <c r="A204" s="7"/>
-      <c r="B204" s="7"/>
-      <c r="C204" s="7"/>
-    </row>
-    <row r="205">
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
+    </row>
+    <row r="204" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A204" s="6"/>
+      <c r="B204" s="6"/>
+      <c r="C204" s="6"/>
+    </row>
+    <row r="205" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B205" s="10"/>
-      <c r="C205" s="10"/>
-      <c r="D205" s="10"/>
-      <c r="E205" s="10"/>
-      <c r="F205" s="10"/>
-      <c r="G205" s="10"/>
-      <c r="H205" s="10"/>
-      <c r="I205" s="10"/>
-      <c r="J205" s="10"/>
-      <c r="K205" s="10"/>
-      <c r="L205" s="10"/>
-      <c r="M205" s="10"/>
-      <c r="N205" s="10"/>
-      <c r="O205" s="10"/>
-      <c r="P205" s="10"/>
-      <c r="Q205" s="10"/>
-      <c r="R205" s="10"/>
-      <c r="S205" s="10"/>
-      <c r="T205" s="10"/>
-      <c r="U205" s="10"/>
-      <c r="V205" s="10"/>
-      <c r="W205" s="10"/>
-      <c r="X205" s="10"/>
-      <c r="Y205" s="10"/>
-      <c r="Z205" s="10"/>
-    </row>
-    <row r="206">
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
+      <c r="E205" s="2"/>
+      <c r="F205" s="2"/>
+      <c r="G205" s="2"/>
+      <c r="H205" s="2"/>
+      <c r="I205" s="2"/>
+      <c r="J205" s="2"/>
+      <c r="K205" s="2"/>
+      <c r="L205" s="2"/>
+      <c r="M205" s="2"/>
+      <c r="N205" s="2"/>
+      <c r="O205" s="2"/>
+      <c r="P205" s="2"/>
+      <c r="Q205" s="2"/>
+      <c r="R205" s="2"/>
+      <c r="S205" s="2"/>
+      <c r="T205" s="2"/>
+      <c r="U205" s="2"/>
+      <c r="V205" s="2"/>
+      <c r="W205" s="2"/>
+      <c r="X205" s="2"/>
+      <c r="Y205" s="2"/>
+      <c r="Z205" s="2"/>
+    </row>
+    <row r="206" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B206" s="7"/>
-      <c r="C206" s="7"/>
-    </row>
-    <row r="207">
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
+    </row>
+    <row r="207" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B207" s="7"/>
-      <c r="C207" s="7"/>
-    </row>
-    <row r="208">
-      <c r="A208" s="7"/>
-      <c r="B208" s="7"/>
-      <c r="C208" s="7"/>
-    </row>
-    <row r="209">
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
+    </row>
+    <row r="208" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A208" s="6"/>
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
+    </row>
+    <row r="209" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B209" s="7"/>
-      <c r="C209" s="7"/>
-    </row>
-    <row r="210">
-      <c r="A210" s="7"/>
-      <c r="B210" s="7"/>
-      <c r="C210" s="7"/>
-    </row>
-    <row r="211">
+      <c r="B209" s="6"/>
+      <c r="C209" s="6"/>
+    </row>
+    <row r="210" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A210" s="6"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="6"/>
+    </row>
+    <row r="211" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="B211" s="7"/>
-      <c r="C211" s="7"/>
-    </row>
-    <row r="212">
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
+    </row>
+    <row r="212" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B212" s="7"/>
-      <c r="C212" s="7"/>
-    </row>
-    <row r="213">
+      <c r="B212" s="6"/>
+      <c r="C212" s="6"/>
+    </row>
+    <row r="213" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B213" s="7"/>
-      <c r="C213" s="7"/>
-    </row>
-    <row r="214">
-      <c r="A214" s="7"/>
-      <c r="B214" s="7"/>
-      <c r="C214" s="7"/>
-    </row>
-    <row r="215">
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
+    </row>
+    <row r="214" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A214" s="6"/>
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+    </row>
+    <row r="215" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B215" s="10"/>
-      <c r="C215" s="10"/>
-      <c r="D215" s="10"/>
-      <c r="E215" s="10"/>
-      <c r="F215" s="10"/>
-      <c r="G215" s="10"/>
-      <c r="H215" s="10"/>
-      <c r="I215" s="10"/>
-      <c r="J215" s="10"/>
-      <c r="K215" s="10"/>
-      <c r="L215" s="10"/>
-      <c r="M215" s="10"/>
-      <c r="N215" s="10"/>
-      <c r="O215" s="10"/>
-      <c r="P215" s="10"/>
-      <c r="Q215" s="10"/>
-      <c r="R215" s="10"/>
-      <c r="S215" s="10"/>
-      <c r="T215" s="10"/>
-      <c r="U215" s="10"/>
-      <c r="V215" s="10"/>
-      <c r="W215" s="10"/>
-      <c r="X215" s="10"/>
-      <c r="Y215" s="10"/>
-      <c r="Z215" s="10"/>
-    </row>
-    <row r="216">
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+      <c r="D215" s="2"/>
+      <c r="E215" s="2"/>
+      <c r="F215" s="2"/>
+      <c r="G215" s="2"/>
+      <c r="H215" s="2"/>
+      <c r="I215" s="2"/>
+      <c r="J215" s="2"/>
+      <c r="K215" s="2"/>
+      <c r="L215" s="2"/>
+      <c r="M215" s="2"/>
+      <c r="N215" s="2"/>
+      <c r="O215" s="2"/>
+      <c r="P215" s="2"/>
+      <c r="Q215" s="2"/>
+      <c r="R215" s="2"/>
+      <c r="S215" s="2"/>
+      <c r="T215" s="2"/>
+      <c r="U215" s="2"/>
+      <c r="V215" s="2"/>
+      <c r="W215" s="2"/>
+      <c r="X215" s="2"/>
+      <c r="Y215" s="2"/>
+      <c r="Z215" s="2"/>
+    </row>
+    <row r="216" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B216" s="7"/>
-      <c r="C216" s="7"/>
-    </row>
-    <row r="217">
+      <c r="B216" s="6"/>
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B217" s="7"/>
-      <c r="C217" s="7"/>
-    </row>
-    <row r="218">
-      <c r="A218" s="7"/>
-      <c r="B218" s="7"/>
-      <c r="C218" s="7"/>
-    </row>
-    <row r="219">
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+    </row>
+    <row r="218" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A218" s="6"/>
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
+    </row>
+    <row r="219" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B219" s="7"/>
-      <c r="C219" s="7"/>
-    </row>
-    <row r="220">
-      <c r="A220" s="7"/>
-      <c r="B220" s="7"/>
-      <c r="C220" s="7"/>
-    </row>
-    <row r="221">
+      <c r="B219" s="6"/>
+      <c r="C219" s="6"/>
+    </row>
+    <row r="220" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A220" s="6"/>
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+    </row>
+    <row r="221" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B221" s="7"/>
-      <c r="C221" s="7"/>
-    </row>
-    <row r="222">
+      <c r="B221" s="6"/>
+      <c r="C221" s="6"/>
+    </row>
+    <row r="222" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A222" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="B222" s="7"/>
-      <c r="C222" s="7"/>
-    </row>
-    <row r="223">
+      <c r="B222" s="6"/>
+      <c r="C222" s="6"/>
+    </row>
+    <row r="223" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A223" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B223" s="7"/>
-      <c r="C223" s="7"/>
-    </row>
-    <row r="224">
-      <c r="A224" s="7"/>
-      <c r="B224" s="7"/>
-      <c r="C224" s="7"/>
-    </row>
-    <row r="225">
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
+    </row>
+    <row r="224" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A224" s="6"/>
+      <c r="B224" s="6"/>
+      <c r="C224" s="6"/>
+    </row>
+    <row r="225" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B225" s="10"/>
-      <c r="C225" s="10"/>
-      <c r="D225" s="10"/>
-      <c r="E225" s="10"/>
-      <c r="F225" s="10"/>
-      <c r="G225" s="10"/>
-      <c r="H225" s="10"/>
-      <c r="I225" s="10"/>
-      <c r="J225" s="10"/>
-      <c r="K225" s="10"/>
-      <c r="L225" s="10"/>
-      <c r="M225" s="10"/>
-      <c r="N225" s="10"/>
-      <c r="O225" s="10"/>
-      <c r="P225" s="10"/>
-      <c r="Q225" s="10"/>
-      <c r="R225" s="10"/>
-      <c r="S225" s="10"/>
-      <c r="T225" s="10"/>
-      <c r="U225" s="10"/>
-      <c r="V225" s="10"/>
-      <c r="W225" s="10"/>
-      <c r="X225" s="10"/>
-      <c r="Y225" s="10"/>
-      <c r="Z225" s="10"/>
-    </row>
-    <row r="226">
+      <c r="B225" s="2"/>
+      <c r="C225" s="2"/>
+      <c r="D225" s="2"/>
+      <c r="E225" s="2"/>
+      <c r="F225" s="2"/>
+      <c r="G225" s="2"/>
+      <c r="H225" s="2"/>
+      <c r="I225" s="2"/>
+      <c r="J225" s="2"/>
+      <c r="K225" s="2"/>
+      <c r="L225" s="2"/>
+      <c r="M225" s="2"/>
+      <c r="N225" s="2"/>
+      <c r="O225" s="2"/>
+      <c r="P225" s="2"/>
+      <c r="Q225" s="2"/>
+      <c r="R225" s="2"/>
+      <c r="S225" s="2"/>
+      <c r="T225" s="2"/>
+      <c r="U225" s="2"/>
+      <c r="V225" s="2"/>
+      <c r="W225" s="2"/>
+      <c r="X225" s="2"/>
+      <c r="Y225" s="2"/>
+      <c r="Z225" s="2"/>
+    </row>
+    <row r="226" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A226" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B226" s="7"/>
-      <c r="C226" s="7"/>
-    </row>
-    <row r="227">
+      <c r="B226" s="6"/>
+      <c r="C226" s="6"/>
+    </row>
+    <row r="227" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B227" s="7"/>
-      <c r="C227" s="7"/>
-    </row>
-    <row r="228">
-      <c r="A228" s="7"/>
-      <c r="B228" s="7"/>
-      <c r="C228" s="7"/>
-    </row>
-    <row r="229">
+      <c r="B227" s="6"/>
+      <c r="C227" s="6"/>
+    </row>
+    <row r="228" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A228" s="6"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="6"/>
+    </row>
+    <row r="229" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A229" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B229" s="7"/>
-      <c r="C229" s="7"/>
-    </row>
-    <row r="230">
-      <c r="A230" s="7"/>
-      <c r="B230" s="7"/>
-      <c r="C230" s="7"/>
-    </row>
-    <row r="231">
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
+    </row>
+    <row r="230" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+      <c r="A230" s="6"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="6"/>
+    </row>
+    <row r="231" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B231" s="7"/>
-      <c r="C231" s="7"/>
-    </row>
-    <row r="232">
+      <c r="B231" s="6"/>
+      <c r="C231" s="6"/>
+    </row>
+    <row r="232" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B232" s="7"/>
-      <c r="C232" s="7"/>
-    </row>
-    <row r="233">
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+    </row>
+    <row r="233" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="B233" s="7"/>
-      <c r="C233" s="7"/>
-    </row>
-    <row r="235">
-      <c r="A235" s="8" t="s">
+      <c r="B233" s="6"/>
+      <c r="C233" s="6"/>
+    </row>
+    <row r="235" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A235" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B235" s="9"/>
-      <c r="C235" s="9"/>
-      <c r="D235" s="9"/>
-      <c r="E235" s="9"/>
-      <c r="F235" s="9"/>
-      <c r="G235" s="9"/>
-      <c r="H235" s="9"/>
-      <c r="I235" s="9"/>
-      <c r="J235" s="9"/>
-      <c r="K235" s="9"/>
-      <c r="L235" s="9"/>
-      <c r="M235" s="9"/>
-      <c r="N235" s="9"/>
-      <c r="O235" s="9"/>
-      <c r="P235" s="9"/>
-      <c r="Q235" s="9"/>
-      <c r="R235" s="9"/>
-      <c r="S235" s="9"/>
-      <c r="T235" s="9"/>
-      <c r="U235" s="9"/>
-      <c r="V235" s="9"/>
-      <c r="W235" s="9"/>
-      <c r="X235" s="9"/>
-      <c r="Y235" s="9"/>
-      <c r="Z235" s="9"/>
-    </row>
-    <row r="237">
+      <c r="B235" s="1"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1"/>
+      <c r="E235" s="1"/>
+      <c r="F235" s="1"/>
+      <c r="G235" s="1"/>
+      <c r="H235" s="1"/>
+      <c r="I235" s="1"/>
+      <c r="J235" s="1"/>
+      <c r="K235" s="1"/>
+      <c r="L235" s="1"/>
+      <c r="M235" s="1"/>
+      <c r="N235" s="1"/>
+      <c r="O235" s="1"/>
+      <c r="P235" s="1"/>
+      <c r="Q235" s="1"/>
+      <c r="R235" s="1"/>
+      <c r="S235" s="1"/>
+      <c r="T235" s="1"/>
+      <c r="U235" s="1"/>
+      <c r="V235" s="1"/>
+      <c r="W235" s="1"/>
+      <c r="X235" s="1"/>
+      <c r="Y235" s="1"/>
+      <c r="Z235" s="1"/>
+    </row>
+    <row r="237" spans="1:26" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B237" s="10"/>
-      <c r="C237" s="10"/>
-      <c r="D237" s="10"/>
-      <c r="E237" s="10"/>
-      <c r="F237" s="10"/>
-      <c r="G237" s="10"/>
-      <c r="H237" s="10"/>
-      <c r="I237" s="10"/>
-      <c r="J237" s="10"/>
-      <c r="K237" s="10"/>
-      <c r="L237" s="10"/>
-      <c r="M237" s="10"/>
-      <c r="N237" s="10"/>
-      <c r="O237" s="10"/>
-      <c r="P237" s="10"/>
-      <c r="Q237" s="10"/>
-      <c r="R237" s="10"/>
-      <c r="S237" s="10"/>
-      <c r="T237" s="10"/>
-      <c r="U237" s="10"/>
-      <c r="V237" s="10"/>
-      <c r="W237" s="10"/>
-      <c r="X237" s="10"/>
-      <c r="Y237" s="10"/>
-      <c r="Z237" s="10"/>
-    </row>
-    <row r="239">
+      <c r="B237" s="2"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+      <c r="E237" s="2"/>
+      <c r="F237" s="2"/>
+      <c r="G237" s="2"/>
+      <c r="H237" s="2"/>
+      <c r="I237" s="2"/>
+      <c r="J237" s="2"/>
+      <c r="K237" s="2"/>
+      <c r="L237" s="2"/>
+      <c r="M237" s="2"/>
+      <c r="N237" s="2"/>
+      <c r="O237" s="2"/>
+      <c r="P237" s="2"/>
+      <c r="Q237" s="2"/>
+      <c r="R237" s="2"/>
+      <c r="S237" s="2"/>
+      <c r="T237" s="2"/>
+      <c r="U237" s="2"/>
+      <c r="V237" s="2"/>
+      <c r="W237" s="2"/>
+      <c r="X237" s="2"/>
+      <c r="Y237" s="2"/>
+      <c r="Z237" s="2"/>
+    </row>
+    <row r="239" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A239" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B239" s="7"/>
-    </row>
-    <row r="240">
+      <c r="B239" s="6"/>
+    </row>
+    <row r="240" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A240" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B240" s="7"/>
-    </row>
-    <row r="241">
-      <c r="A241" s="7"/>
-      <c r="B241" s="7"/>
-    </row>
-    <row r="242">
+      <c r="B240" s="6"/>
+    </row>
+    <row r="241" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A241" s="6"/>
+      <c r="B241" s="6"/>
+    </row>
+    <row r="242" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A242" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B242" s="7"/>
-    </row>
-    <row r="243">
+      <c r="B242" s="6"/>
+    </row>
+    <row r="243" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A243" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="B243" s="7"/>
-    </row>
-    <row r="244">
-      <c r="A244" s="7"/>
-      <c r="B244" s="7"/>
-    </row>
-    <row r="245">
+      <c r="B243" s="6"/>
+    </row>
+    <row r="244" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A244" s="6"/>
+      <c r="B244" s="6"/>
+    </row>
+    <row r="245" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A245" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B245" s="7"/>
-    </row>
-    <row r="246">
+      <c r="B245" s="6"/>
+    </row>
+    <row r="246" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A246" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B246" s="7"/>
-    </row>
-    <row r="247">
-      <c r="A247" s="7"/>
-      <c r="B247" s="7"/>
-    </row>
-    <row r="248">
+      <c r="B246" s="6"/>
+    </row>
+    <row r="247" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A247" s="6"/>
+      <c r="B247" s="6"/>
+    </row>
+    <row r="248" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A248" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B248" s="7"/>
-    </row>
-    <row r="249">
-      <c r="A249" s="7"/>
-      <c r="B249" s="7"/>
-    </row>
-    <row r="250">
+      <c r="B248" s="6"/>
+    </row>
+    <row r="249" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A249" s="6"/>
+      <c r="B249" s="6"/>
+    </row>
+    <row r="250" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A250" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B250" s="7"/>
-    </row>
-    <row r="251">
-      <c r="A251" s="7"/>
-      <c r="B251" s="7"/>
-    </row>
-    <row r="252">
+      <c r="B250" s="6"/>
+    </row>
+    <row r="251" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A251" s="6"/>
+      <c r="B251" s="6"/>
+    </row>
+    <row r="252" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A252" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="B252" s="7"/>
-    </row>
-    <row r="253">
-      <c r="A253" s="7"/>
-      <c r="B253" s="7"/>
-    </row>
-    <row r="254">
+      <c r="B252" s="6"/>
+    </row>
+    <row r="253" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A253" s="6"/>
+      <c r="B253" s="6"/>
+    </row>
+    <row r="254" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A254" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="B254" s="7"/>
-    </row>
-    <row r="255">
-      <c r="A255" s="7"/>
-      <c r="B255" s="7"/>
-    </row>
-    <row r="256">
+      <c r="B254" s="6"/>
+    </row>
+    <row r="255" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A255" s="6"/>
+      <c r="B255" s="6"/>
+    </row>
+    <row r="256" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A256" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="B256" s="7"/>
-    </row>
-    <row r="257">
+      <c r="B256" s="6"/>
+    </row>
+    <row r="257" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A257" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B257" s="7"/>
-    </row>
-    <row r="258">
-      <c r="A258" s="7"/>
-      <c r="B258" s="7"/>
-    </row>
-    <row r="259">
+      <c r="B257" s="6"/>
+    </row>
+    <row r="258" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A258" s="6"/>
+      <c r="B258" s="6"/>
+    </row>
+    <row r="259" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A259" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="B259" s="7"/>
-    </row>
-    <row r="260">
+      <c r="B259" s="6"/>
+    </row>
+    <row r="260" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A260" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="B260" s="7"/>
-    </row>
-    <row r="261">
-      <c r="A261" s="7"/>
-      <c r="B261" s="7"/>
-    </row>
-    <row r="262">
+      <c r="B260" s="6"/>
+    </row>
+    <row r="261" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A261" s="6"/>
+      <c r="B261" s="6"/>
+    </row>
+    <row r="262" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A262" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B262" s="7"/>
-    </row>
-    <row r="263">
-      <c r="A263" s="7"/>
-      <c r="B263" s="7"/>
-    </row>
-    <row r="264">
+      <c r="B262" s="6"/>
+    </row>
+    <row r="263" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A263" s="6"/>
+      <c r="B263" s="6"/>
+    </row>
+    <row r="264" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A264" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B264" s="7"/>
-    </row>
-    <row r="265">
-      <c r="A265" s="7"/>
-      <c r="B265" s="7"/>
-    </row>
-    <row r="266">
+      <c r="B264" s="6"/>
+    </row>
+    <row r="265" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A265" s="6"/>
+      <c r="B265" s="6"/>
+    </row>
+    <row r="266" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A266" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B266" s="7"/>
-    </row>
-    <row r="267">
-      <c r="A267" s="7"/>
-      <c r="B267" s="7"/>
-    </row>
-    <row r="268">
+      <c r="B266" s="6"/>
+    </row>
+    <row r="267" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A267" s="6"/>
+      <c r="B267" s="6"/>
+    </row>
+    <row r="268" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A268" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B268" s="7"/>
-    </row>
-    <row r="269">
-      <c r="A269" s="7"/>
-      <c r="B269" s="7"/>
-    </row>
-    <row r="270">
+      <c r="B268" s="6"/>
+    </row>
+    <row r="269" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A269" s="6"/>
+      <c r="B269" s="6"/>
+    </row>
+    <row r="270" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A270" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="B270" s="7"/>
-    </row>
-    <row r="271">
-      <c r="A271" s="7"/>
-      <c r="B271" s="7"/>
-    </row>
-    <row r="272">
+      <c r="B270" s="6"/>
+    </row>
+    <row r="271" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A271" s="6"/>
+      <c r="B271" s="6"/>
+    </row>
+    <row r="272" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A272" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B272" s="7"/>
-    </row>
-    <row r="273">
-      <c r="A273" s="7"/>
-      <c r="B273" s="7"/>
-    </row>
-    <row r="274">
+      <c r="B272" s="6"/>
+    </row>
+    <row r="273" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A273" s="6"/>
+      <c r="B273" s="6"/>
+    </row>
+    <row r="274" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A274" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="B274" s="7"/>
-    </row>
-    <row r="275">
+      <c r="B274" s="6"/>
+    </row>
+    <row r="275" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A275" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B275" s="7"/>
-    </row>
-    <row r="276">
-      <c r="A276" s="7"/>
-      <c r="B276" s="7"/>
-    </row>
-    <row r="277">
+      <c r="B275" s="6"/>
+    </row>
+    <row r="276" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A276" s="6"/>
+      <c r="B276" s="6"/>
+    </row>
+    <row r="277" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A277" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B277" s="7"/>
-    </row>
-    <row r="278">
+      <c r="B277" s="6"/>
+    </row>
+    <row r="278" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A278" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B278" s="7"/>
-    </row>
-    <row r="279">
-      <c r="A279" s="7"/>
-      <c r="B279" s="7"/>
-    </row>
-    <row r="280">
+      <c r="B278" s="6"/>
+    </row>
+    <row r="279" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A279" s="6"/>
+      <c r="B279" s="6"/>
+    </row>
+    <row r="280" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A280" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B280" s="7"/>
-    </row>
-    <row r="281">
+      <c r="B280" s="6"/>
+    </row>
+    <row r="281" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A281" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B281" s="7"/>
-    </row>
-    <row r="282">
-      <c r="A282" s="7"/>
-      <c r="B282" s="7"/>
-    </row>
-    <row r="283">
+      <c r="B281" s="6"/>
+    </row>
+    <row r="282" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A282" s="6"/>
+      <c r="B282" s="6"/>
+    </row>
+    <row r="283" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A283" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B283" s="7"/>
-    </row>
-    <row r="284">
+      <c r="B283" s="6"/>
+    </row>
+    <row r="284" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A284" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B284" s="7"/>
-    </row>
-    <row r="285">
-      <c r="A285" s="7"/>
-      <c r="B285" s="7"/>
-    </row>
-    <row r="286">
+      <c r="B284" s="6"/>
+    </row>
+    <row r="285" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A285" s="6"/>
+      <c r="B285" s="6"/>
+    </row>
+    <row r="286" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A286" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B286" s="7"/>
-    </row>
-    <row r="287">
+      <c r="B286" s="6"/>
+    </row>
+    <row r="287" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A287" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B287" s="7"/>
-    </row>
-    <row r="288">
-      <c r="A288" s="7"/>
-      <c r="B288" s="7"/>
-    </row>
-    <row r="289">
+      <c r="B287" s="6"/>
+    </row>
+    <row r="288" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A288" s="6"/>
+      <c r="B288" s="6"/>
+    </row>
+    <row r="289" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A289" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B289" s="7"/>
-    </row>
-    <row r="290">
+      <c r="B289" s="6"/>
+    </row>
+    <row r="290" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A290" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B290" s="7"/>
-    </row>
-    <row r="292">
-      <c r="A292" s="8" t="s">
+      <c r="B290" s="6"/>
+    </row>
+    <row r="292" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A292" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B292" s="9"/>
-      <c r="C292" s="9"/>
-      <c r="D292" s="9"/>
-      <c r="E292" s="9"/>
-      <c r="F292" s="9"/>
-      <c r="G292" s="9"/>
-      <c r="H292" s="9"/>
-      <c r="I292" s="9"/>
-      <c r="J292" s="9"/>
-      <c r="K292" s="9"/>
-      <c r="L292" s="9"/>
-      <c r="M292" s="9"/>
-      <c r="N292" s="9"/>
-      <c r="O292" s="9"/>
-      <c r="P292" s="9"/>
-      <c r="Q292" s="9"/>
-      <c r="R292" s="9"/>
-      <c r="S292" s="9"/>
-      <c r="T292" s="9"/>
-      <c r="U292" s="9"/>
-      <c r="V292" s="9"/>
-      <c r="W292" s="9"/>
-      <c r="X292" s="9"/>
-      <c r="Y292" s="9"/>
-      <c r="Z292" s="9"/>
-    </row>
-    <row r="294">
+      <c r="B292" s="1"/>
+      <c r="C292" s="1"/>
+      <c r="D292" s="1"/>
+      <c r="E292" s="1"/>
+      <c r="F292" s="1"/>
+      <c r="G292" s="1"/>
+      <c r="H292" s="1"/>
+      <c r="I292" s="1"/>
+      <c r="J292" s="1"/>
+      <c r="K292" s="1"/>
+      <c r="L292" s="1"/>
+      <c r="M292" s="1"/>
+      <c r="N292" s="1"/>
+      <c r="O292" s="1"/>
+      <c r="P292" s="1"/>
+      <c r="Q292" s="1"/>
+      <c r="R292" s="1"/>
+      <c r="S292" s="1"/>
+      <c r="T292" s="1"/>
+      <c r="U292" s="1"/>
+      <c r="V292" s="1"/>
+      <c r="W292" s="1"/>
+      <c r="X292" s="1"/>
+      <c r="Y292" s="1"/>
+      <c r="Z292" s="1"/>
+    </row>
+    <row r="294" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A294" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="B294" s="7"/>
-      <c r="C294" s="7"/>
-    </row>
-    <row r="295">
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
+    </row>
+    <row r="295" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A295" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="B295" s="7"/>
-      <c r="C295" s="7"/>
-    </row>
-    <row r="296">
+      <c r="B295" s="6"/>
+      <c r="C295" s="6"/>
+    </row>
+    <row r="296" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A296" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B296" s="7"/>
-      <c r="C296" s="7"/>
-    </row>
-    <row r="297">
+      <c r="B296" s="6"/>
+      <c r="C296" s="6"/>
+    </row>
+    <row r="297" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A297" s="6"/>
-      <c r="B297" s="7"/>
-      <c r="C297" s="7"/>
-    </row>
-    <row r="298">
+      <c r="B297" s="6"/>
+      <c r="C297" s="6"/>
+    </row>
+    <row r="298" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A298" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="B298" s="7"/>
-      <c r="C298" s="7"/>
-    </row>
-    <row r="299">
+      <c r="B298" s="6"/>
+      <c r="C298" s="6"/>
+    </row>
+    <row r="299" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A299" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="B299" s="7"/>
-      <c r="C299" s="7"/>
-    </row>
-    <row r="300">
+      <c r="B299" s="6"/>
+      <c r="C299" s="6"/>
+    </row>
+    <row r="300" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A300" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="B300" s="7"/>
-      <c r="C300" s="7"/>
-    </row>
-    <row r="301">
+      <c r="B300" s="6"/>
+      <c r="C300" s="6"/>
+    </row>
+    <row r="301" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A301" s="6"/>
-      <c r="B301" s="7"/>
-      <c r="C301" s="7"/>
-    </row>
-    <row r="302">
+      <c r="B301" s="6"/>
+      <c r="C301" s="6"/>
+    </row>
+    <row r="302" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A302" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B302" s="7"/>
-      <c r="C302" s="7"/>
-    </row>
-    <row r="303">
+      <c r="B302" s="6"/>
+      <c r="C302" s="6"/>
+    </row>
+    <row r="303" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A303" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B303" s="7"/>
-      <c r="C303" s="7"/>
-    </row>
-    <row r="304">
+      <c r="B303" s="6"/>
+      <c r="C303" s="6"/>
+    </row>
+    <row r="304" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A304" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B304" s="7"/>
-      <c r="C304" s="7"/>
-    </row>
-    <row r="305">
+      <c r="B304" s="6"/>
+      <c r="C304" s="6"/>
+    </row>
+    <row r="305" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A305" s="6"/>
-      <c r="B305" s="7"/>
-      <c r="C305" s="7"/>
-    </row>
-    <row r="306">
+      <c r="B305" s="6"/>
+      <c r="C305" s="6"/>
+    </row>
+    <row r="306" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A306" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="B306" s="7"/>
-      <c r="C306" s="7"/>
-    </row>
-    <row r="307">
+      <c r="B306" s="6"/>
+      <c r="C306" s="6"/>
+    </row>
+    <row r="307" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A307" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="B307" s="7"/>
-      <c r="C307" s="7"/>
-    </row>
-    <row r="308">
+      <c r="B307" s="6"/>
+      <c r="C307" s="6"/>
+    </row>
+    <row r="308" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A308" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B308" s="7"/>
-      <c r="C308" s="7"/>
-    </row>
-    <row r="309">
+      <c r="B308" s="6"/>
+      <c r="C308" s="6"/>
+    </row>
+    <row r="309" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A309" s="6"/>
-      <c r="B309" s="7"/>
-      <c r="C309" s="7"/>
-    </row>
-    <row r="310">
+      <c r="B309" s="6"/>
+      <c r="C309" s="6"/>
+    </row>
+    <row r="310" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A310" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B310" s="7"/>
-      <c r="C310" s="7"/>
-    </row>
-    <row r="311">
+      <c r="B310" s="6"/>
+      <c r="C310" s="6"/>
+    </row>
+    <row r="311" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A311" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B311" s="7"/>
-      <c r="C311" s="7"/>
-    </row>
-    <row r="312">
+      <c r="B311" s="6"/>
+      <c r="C311" s="6"/>
+    </row>
+    <row r="312" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A312" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B312" s="7"/>
-      <c r="C312" s="7"/>
-    </row>
-    <row r="313">
+      <c r="B312" s="6"/>
+      <c r="C312" s="6"/>
+    </row>
+    <row r="313" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A313" s="6"/>
-      <c r="B313" s="7"/>
-      <c r="C313" s="7"/>
-    </row>
-    <row r="314">
+      <c r="B313" s="6"/>
+      <c r="C313" s="6"/>
+    </row>
+    <row r="314" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A314" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="B314" s="7"/>
-      <c r="C314" s="7"/>
-    </row>
-    <row r="315">
+      <c r="B314" s="6"/>
+      <c r="C314" s="6"/>
+    </row>
+    <row r="315" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A315" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B315" s="7"/>
-      <c r="C315" s="7"/>
-    </row>
-    <row r="316">
+      <c r="B315" s="6"/>
+      <c r="C315" s="6"/>
+    </row>
+    <row r="316" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A316" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B316" s="7"/>
-      <c r="C316" s="7"/>
-    </row>
-    <row r="317">
+      <c r="B316" s="6"/>
+      <c r="C316" s="6"/>
+    </row>
+    <row r="317" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A317" s="6"/>
-      <c r="B317" s="7"/>
-      <c r="C317" s="7"/>
-    </row>
-    <row r="318">
+      <c r="B317" s="6"/>
+      <c r="C317" s="6"/>
+    </row>
+    <row r="318" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A318" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B318" s="7"/>
-      <c r="C318" s="7"/>
-    </row>
-    <row r="319">
+      <c r="B318" s="6"/>
+      <c r="C318" s="6"/>
+    </row>
+    <row r="319" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A319" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B319" s="7"/>
-      <c r="C319" s="7"/>
-    </row>
-    <row r="320">
+      <c r="B319" s="6"/>
+      <c r="C319" s="6"/>
+    </row>
+    <row r="320" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A320" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B320" s="7"/>
-      <c r="C320" s="7"/>
-    </row>
-    <row r="321">
+      <c r="B320" s="6"/>
+      <c r="C320" s="6"/>
+    </row>
+    <row r="321" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A321" s="6"/>
-      <c r="B321" s="7"/>
-      <c r="C321" s="7"/>
-    </row>
-    <row r="322">
+      <c r="B321" s="6"/>
+      <c r="C321" s="6"/>
+    </row>
+    <row r="322" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A322" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B322" s="7"/>
-      <c r="C322" s="7"/>
-    </row>
-    <row r="323">
+      <c r="B322" s="6"/>
+      <c r="C322" s="6"/>
+    </row>
+    <row r="323" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A323" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B323" s="7"/>
-      <c r="C323" s="7"/>
-    </row>
-    <row r="324">
+      <c r="B323" s="6"/>
+      <c r="C323" s="6"/>
+    </row>
+    <row r="324" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A324" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B324" s="7"/>
-      <c r="C324" s="7"/>
-    </row>
-    <row r="325">
+      <c r="B324" s="6"/>
+      <c r="C324" s="6"/>
+    </row>
+    <row r="325" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A325" s="6"/>
-      <c r="B325" s="7"/>
-      <c r="C325" s="7"/>
-    </row>
-    <row r="326">
+      <c r="B325" s="6"/>
+      <c r="C325" s="6"/>
+    </row>
+    <row r="326" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A326" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B326" s="7"/>
-      <c r="C326" s="7"/>
-    </row>
-    <row r="327">
+      <c r="B326" s="6"/>
+      <c r="C326" s="6"/>
+    </row>
+    <row r="327" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A327" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B327" s="7"/>
-      <c r="C327" s="7"/>
-    </row>
-    <row r="328">
+      <c r="B327" s="6"/>
+      <c r="C327" s="6"/>
+    </row>
+    <row r="328" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A328" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B328" s="7"/>
-      <c r="C328" s="7"/>
-    </row>
-    <row r="329">
+      <c r="B328" s="6"/>
+      <c r="C328" s="6"/>
+    </row>
+    <row r="329" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A329" s="6"/>
-      <c r="B329" s="7"/>
-      <c r="C329" s="7"/>
-    </row>
-    <row r="330">
+      <c r="B329" s="6"/>
+      <c r="C329" s="6"/>
+    </row>
+    <row r="330" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A330" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B330" s="7"/>
-      <c r="C330" s="7"/>
-    </row>
-    <row r="331">
+      <c r="B330" s="6"/>
+      <c r="C330" s="6"/>
+    </row>
+    <row r="331" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A331" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B331" s="7"/>
-      <c r="C331" s="7"/>
-    </row>
-    <row r="332">
+      <c r="B331" s="6"/>
+      <c r="C331" s="6"/>
+    </row>
+    <row r="332" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A332" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B332" s="7"/>
-      <c r="C332" s="7"/>
-    </row>
-    <row r="333">
+      <c r="B332" s="6"/>
+      <c r="C332" s="6"/>
+    </row>
+    <row r="333" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A333" s="6"/>
-      <c r="B333" s="7"/>
-      <c r="C333" s="7"/>
-    </row>
-    <row r="334">
+      <c r="B333" s="6"/>
+      <c r="C333" s="6"/>
+    </row>
+    <row r="334" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A334" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B334" s="7"/>
-      <c r="C334" s="7"/>
-    </row>
-    <row r="335">
+      <c r="B334" s="6"/>
+      <c r="C334" s="6"/>
+    </row>
+    <row r="335" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A335" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B335" s="7"/>
-      <c r="C335" s="7"/>
-    </row>
-    <row r="336">
+      <c r="B335" s="6"/>
+      <c r="C335" s="6"/>
+    </row>
+    <row r="336" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A336" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B336" s="7"/>
-      <c r="C336" s="7"/>
+      <c r="B336" s="6"/>
+      <c r="C336" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:Z1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>